<commit_message>
sprint 5 all changes
</commit_message>
<xml_diff>
--- a/webdata/Offers.xlsx
+++ b/webdata/Offers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0216779/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BAFC60F-3DCC-5941-900A-46610853E163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27445832-3BAC-BD41-882A-ADED11FDC9EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{5820AB65-6943-1149-9D8F-0AEC086C01B5}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{5820AB65-6943-1149-9D8F-0AEC086C01B5}"/>
   </bookViews>
   <sheets>
     <sheet name="BestOffers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>MSISDN</t>
   </si>
@@ -58,6 +58,9 @@
     <t>PREPAID</t>
   </si>
   <si>
+    <t>755841007</t>
+  </si>
+  <si>
     <t>Commission(Percentage)</t>
   </si>
   <si>
@@ -70,7 +73,10 @@
     <t>100</t>
   </si>
   <si>
-    <t>POSTPAID</t>
+    <t>99</t>
+  </si>
+  <si>
+    <t>PREPAID (OR) POSTPAID</t>
   </si>
 </sst>
 </file>
@@ -129,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -143,6 +149,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED2D1F-8AF8-A446-8673-D75B162E1B35}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +492,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -496,8 +503,8 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>753011515</v>
+      <c r="A2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
@@ -506,18 +513,19 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>755843100</v>
+      <c r="A3" s="1">
+        <v>755841007</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -526,14 +534,36 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>755841651</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>